<commit_message>
java version changed to 17
</commit_message>
<xml_diff>
--- a/src/test/java/inputFiles/sauceInputFile.xlsx
+++ b/src/test/java/inputFiles/sauceInputFile.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25726"/>
   <workbookPr/>
-  <mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\akula\IdeaProjects\ShoppingKartProject\src\test\java\inputFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F70007F-589F-4FB3-B9E8-EE9119A5ADB2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43448EAC-575F-4AF4-976A-18F29ABE954F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1920" yWindow="1920" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -17,7 +17,7 @@
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -25,67 +25,60 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="16">
   <si>
     <t>Item1</t>
   </si>
   <si>
+    <t>Item3</t>
+  </si>
+  <si>
+    <t>firstName</t>
+  </si>
+  <si>
+    <t>lastName</t>
+  </si>
+  <si>
+    <t>zipCode</t>
+  </si>
+  <si>
+    <t>itemTotal</t>
+  </si>
+  <si>
+    <t>Tax</t>
+  </si>
+  <si>
+    <t>Total</t>
+  </si>
+  <si>
+    <t>backpack</t>
+  </si>
+  <si>
+    <t>tshirt</t>
+  </si>
+  <si>
+    <t>bikelight</t>
+  </si>
+  <si>
+    <t>max</t>
+  </si>
+  <si>
+    <t>planck</t>
+  </si>
+  <si>
+    <t>edward</t>
+  </si>
+  <si>
+    <t>snowden</t>
+  </si>
+  <si>
     <t>Item2</t>
-  </si>
-  <si>
-    <t>Item3</t>
-  </si>
-  <si>
-    <t>firstName</t>
-  </si>
-  <si>
-    <t>lastName</t>
-  </si>
-  <si>
-    <t>zipCode</t>
-  </si>
-  <si>
-    <t>itemTotal</t>
-  </si>
-  <si>
-    <t>Tax</t>
-  </si>
-  <si>
-    <t>Total</t>
-  </si>
-  <si>
-    <t>backpack</t>
-  </si>
-  <si>
-    <t>bikelight</t>
-  </si>
-  <si>
-    <t>pvn</t>
-  </si>
-  <si>
-    <t>ak</t>
-  </si>
-  <si>
-    <t>max</t>
-  </si>
-  <si>
-    <t>vs</t>
-  </si>
-  <si>
-    <t>$39.98</t>
-  </si>
-  <si>
-    <t>$3.20</t>
-  </si>
-  <si>
-    <t>$43.18</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="0"/>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -400,90 +393,75 @@
   <dimension ref="A1:I3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+      <selection activeCell="G2" sqref="G2:I3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A1" t="s" s="0">
+      <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s" s="0">
+      <c r="B1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s" s="0">
+      <c r="D1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s" s="0">
+      <c r="E1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s" s="0">
+      <c r="F1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s" s="0">
+      <c r="G1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s" s="0">
+      <c r="H1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s" s="0">
+      <c r="I1" t="s">
         <v>7</v>
-      </c>
-      <c r="I1" t="s" s="0">
-        <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A2" t="s" s="0">
+      <c r="A2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" t="s">
         <v>9</v>
       </c>
-      <c r="B2" t="s" s="0">
+      <c r="C2" t="s">
         <v>10</v>
       </c>
-      <c r="D2" t="s" s="0">
+      <c r="D2" t="s">
         <v>11</v>
       </c>
-      <c r="E2" t="s" s="0">
+      <c r="E2" t="s">
         <v>12</v>
       </c>
-      <c r="F2" s="0">
-        <v>507165</v>
-      </c>
-      <c r="G2" t="s" s="0">
-        <v>15</v>
-      </c>
-      <c r="H2" t="s" s="0">
-        <v>16</v>
-      </c>
-      <c r="I2" t="s" s="0">
-        <v>17</v>
+      <c r="F2">
+        <v>722036</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A3" t="s" s="0">
+      <c r="B3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" t="s">
         <v>10</v>
       </c>
-      <c r="B3" t="s" s="0">
-        <v>9</v>
-      </c>
-      <c r="D3" t="s" s="0">
+      <c r="D3" t="s">
         <v>13</v>
       </c>
-      <c r="E3" t="s" s="0">
+      <c r="E3" t="s">
         <v>14</v>
       </c>
-      <c r="F3" s="0">
-        <v>124587</v>
-      </c>
-      <c r="G3" t="s" s="0">
-        <v>15</v>
-      </c>
-      <c r="H3" t="s" s="0">
-        <v>16</v>
-      </c>
-      <c r="I3" t="s" s="0">
-        <v>17</v>
+      <c r="F3">
+        <v>753651</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
driver changed to chrome
</commit_message>
<xml_diff>
--- a/src/test/java/inputFiles/sauceInputFile.xlsx
+++ b/src/test/java/inputFiles/sauceInputFile.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25726"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\akula\IdeaProjects\ShoppingKartProject\src\test\java\inputFiles\"/>
     </mc:Choice>
@@ -17,7 +17,7 @@
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="22">
   <si>
     <t>Item1</t>
   </si>
@@ -73,12 +73,31 @@
   </si>
   <si>
     <t>Item2</t>
+  </si>
+  <si>
+    <t>$55.97</t>
+  </si>
+  <si>
+    <t>$4.48</t>
+  </si>
+  <si>
+    <t>$60.45</t>
+  </si>
+  <si>
+    <t>$25.98</t>
+  </si>
+  <si>
+    <t>$2.08</t>
+  </si>
+  <si>
+    <t>$28.06</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="0"/>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -399,69 +418,87 @@
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
+      <c r="A1" t="s" s="0">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" t="s" s="0">
         <v>15</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" t="s" s="0">
         <v>1</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" t="s" s="0">
         <v>2</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" t="s" s="0">
         <v>3</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" t="s" s="0">
         <v>4</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" t="s" s="0">
         <v>5</v>
       </c>
-      <c r="H1" t="s">
+      <c r="H1" t="s" s="0">
         <v>6</v>
       </c>
-      <c r="I1" t="s">
+      <c r="I1" t="s" s="0">
         <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
+      <c r="A2" t="s" s="0">
         <v>8</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" t="s" s="0">
         <v>9</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" t="s" s="0">
         <v>10</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" t="s" s="0">
         <v>11</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E2" t="s" s="0">
         <v>12</v>
       </c>
-      <c r="F2">
+      <c r="F2" s="0">
         <v>722036</v>
+      </c>
+      <c r="G2" t="s" s="0">
+        <v>16</v>
+      </c>
+      <c r="H2" t="s" s="0">
+        <v>17</v>
+      </c>
+      <c r="I2" t="s" s="0">
+        <v>18</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="B3" t="s">
+      <c r="B3" t="s" s="0">
         <v>9</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" t="s" s="0">
         <v>10</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" t="s" s="0">
         <v>13</v>
       </c>
-      <c r="E3" t="s">
+      <c r="E3" t="s" s="0">
         <v>14</v>
       </c>
-      <c r="F3">
+      <c r="F3" s="0">
         <v>753651</v>
+      </c>
+      <c r="G3" t="s" s="0">
+        <v>19</v>
+      </c>
+      <c r="H3" t="s" s="0">
+        <v>20</v>
+      </c>
+      <c r="I3" t="s" s="0">
+        <v>21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>